<commit_message>
added three more polymerases
</commit_message>
<xml_diff>
--- a/data/combined_polymerases.xlsx
+++ b/data/combined_polymerases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idamei/wzy_polymerases/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3853722A-7A16-7A4E-923F-5657130A8468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4C2DC8-2ED9-B347-8654-B83FEFD42B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="1413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="1425">
   <si>
     <t>species</t>
   </si>
@@ -4259,13 +4259,49 @@
   </si>
   <si>
     <t>MNMTIFIAIIMLMYSGLLLSINKDIKSPSAILFFIWGGLLFLSGVNGDITNYTLCIILFSCLSFSVGALLAKPYAPIFEHVFSYNINNTKALVLITNIISFVILIYTLIVFLYYYKGGFTESYINSRTEINYGDKSGLIKIYGYIYYLLYPLVYVWSFLYFKNKYKKIEEGERARLPYNNRTFYFVFFTSLFYALLSTAKIKVLLLIIPIVFLRLFFQKISLKYLLVTVSGIIFFFYLSMLFLNKIDDSSGAFEALKYGLMNYSLANIFALDSVLQGKAVVIDCNGDATCGLANFISYKEYKTNVFTIFYSLTKYSDFLYSLIFFFVIGFFHSSLYNVAKKNKKTISVVICSILYFPLLFQFFDQLYMLMFYIYAIAMLYVICFCSRLTLTLKGV</t>
+  </si>
+  <si>
+    <t>AAD45264.1</t>
+  </si>
+  <si>
+    <t>Pseudomonas aeruginosa</t>
+  </si>
+  <si>
+    <t>MKQRSVALVLLFVFLFHILRNLSGAYYLVLAGFCGLFFLLFINNWRDIKYSALGIFVIFFWTYASLVSVLWFDLYGDYSIGIFRLWASLPLLFVAMVLARDNLKVPMQLISFFFSLAALSFLWQYVFGPIEWFAEASERAGGARFASLVGSLTAYGVMVGVPALASLFYLKGWARVVCFLLLCLGAMLSLQKAALANIVIVLFFAYWLKLIKKTYLFFTFLLAGLGLSVFFLADFGAGSLETVHRLIVGLLTSDSSVSQDVPFFESIFDRVTALPLETLSFYGSEILVLGAGVFGGGGVLGYAQYPMAHNGIVELLCIYGFIFGGLAVLLLLLLFVYSVFLLVFRRRKTACTELGFLCSAFIIWFVNYVFSGGGLFHPVGAALFWLVVFRFLYILRRKRDVEHISKEVVYG</t>
+  </si>
+  <si>
+    <t>PA103</t>
+  </si>
+  <si>
+    <t>AF147795_5</t>
+  </si>
+  <si>
+    <t>WP_000905563.1</t>
+  </si>
+  <si>
+    <t>Salmonella enterica</t>
+  </si>
+  <si>
+    <t>Typhii</t>
+  </si>
+  <si>
+    <t>CT18</t>
+  </si>
+  <si>
+    <t>MLIISYIALCLLFIVYLYTLSVRIEGKIINVMVPYLIITVPTLYVFEGIFVYLSEVQNYTVEYLFFYTCYITYIASFVISYLYTQRKPIYNKSNTKNKPRYVFTSLLFTFLAFIIYLPVLMEFREYILSPRRIYELTRTGYGIYFYPSLMFSLVASICAFFTYKKSKLFCISIVLFNCILIFLHGNKGPIFSIFIAFILYLSYIENKKIKFMFLVKSFAVIAVIVTAFFAYTFTDGNPIENMANYSDYTRNAVLVASSNFDFMYGKLLMESEVYSRIPRAIWPDKPEDFGALYLAKVFFPDAFYRNQGAPAFGYGELYADFGLFTPVWLVISGVFKGVLAKYFSNKTQETKSAHYFIMFLFCIGISVIPVSMGWLFPEHLMIAFMVYIASSFVFSEHIRFVLLRNNK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WP_000220864.1 </t>
+  </si>
+  <si>
+    <t>MTYFTGFILILFAIIIKRLTPSQSKKNIVLIANAFWGILLVGYAFNEQYFVPLSATTLFFILAFLFFFSMTYILIARSGRVVFSFGTGFIESKYIYWFAGMINIISICFGIILLYNNHFSLKVMREGILDGSISGFGLGISLPLSFCCMYLARHENKKNYFYCFTLLSFLLAVLSTSKIFLILFLVYIVGINSYVSKKKLLIYGVFVFGLFALSSIILGKFSSDPEGKIISAIFDTLRVYLFSGLAAFNLYVEKNATLPENLLLYPFKEVWGTTKDIPKTDILPWINIGVWDTNVYTAFAPWYQSLGLYAAIIIGILLGFYYGIWFSFRQNLAVGFYQTFLCFPLLMLFFQEHYLLSWKMHFIYFLCAILLAMRKALEYE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4283,6 +4319,12 @@
       <color rgb="FF000000"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -4320,12 +4362,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4628,15 +4672,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L384"/>
+  <dimension ref="A1:L387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A341" workbookViewId="0">
-      <selection activeCell="B348" sqref="B348"/>
+    <sheetView tabSelected="1" topLeftCell="A367" workbookViewId="0">
+      <selection activeCell="H389" sqref="H389"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4674,7 +4718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4706,7 +4750,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4741,7 +4785,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4764,7 +4808,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -4787,7 +4831,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4822,7 +4866,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4845,7 +4889,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -4877,7 +4921,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -4900,7 +4944,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -4932,7 +4976,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -4967,7 +5011,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -5002,7 +5046,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -5034,7 +5078,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -5057,7 +5101,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -5080,7 +5124,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -5103,7 +5147,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -5135,7 +5179,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -5158,7 +5202,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -5193,7 +5237,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -5216,7 +5260,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -5239,7 +5283,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -5262,7 +5306,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -5294,7 +5338,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -5329,7 +5373,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -5364,7 +5408,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>12</v>
       </c>
@@ -5387,7 +5431,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -5410,7 +5454,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -5433,7 +5477,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>193</v>
       </c>
@@ -5462,7 +5506,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>193</v>
       </c>
@@ -5491,7 +5535,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>193</v>
       </c>
@@ -5514,7 +5558,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>193</v>
       </c>
@@ -5534,7 +5578,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>193</v>
       </c>
@@ -5563,7 +5607,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>193</v>
       </c>
@@ -5592,7 +5636,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>193</v>
       </c>
@@ -5621,7 +5665,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>193</v>
       </c>
@@ -5650,7 +5694,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>193</v>
       </c>
@@ -5679,7 +5723,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>193</v>
       </c>
@@ -5708,7 +5752,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>193</v>
       </c>
@@ -5737,7 +5781,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>193</v>
       </c>
@@ -5766,7 +5810,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>193</v>
       </c>
@@ -5795,7 +5839,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>193</v>
       </c>
@@ -5824,7 +5868,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>193</v>
       </c>
@@ -5853,7 +5897,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>193</v>
       </c>
@@ -5882,7 +5926,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>193</v>
       </c>
@@ -5911,7 +5955,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
         <v>193</v>
       </c>
@@ -5940,7 +5984,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
         <v>193</v>
       </c>
@@ -5969,7 +6013,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>193</v>
       </c>
@@ -5998,7 +6042,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>193</v>
       </c>
@@ -6027,7 +6071,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
         <v>193</v>
       </c>
@@ -6056,7 +6100,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>193</v>
       </c>
@@ -6085,7 +6129,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>193</v>
       </c>
@@ -6114,7 +6158,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>193</v>
       </c>
@@ -6143,7 +6187,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>193</v>
       </c>
@@ -6172,7 +6216,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12">
       <c r="A55" t="s">
         <v>193</v>
       </c>
@@ -6201,7 +6245,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
         <v>193</v>
       </c>
@@ -6221,7 +6265,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
         <v>193</v>
       </c>
@@ -6250,7 +6294,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
         <v>193</v>
       </c>
@@ -6279,7 +6323,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
         <v>193</v>
       </c>
@@ -6308,7 +6352,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
         <v>193</v>
       </c>
@@ -6337,7 +6381,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
         <v>193</v>
       </c>
@@ -6366,7 +6410,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
         <v>193</v>
       </c>
@@ -6395,7 +6439,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
         <v>193</v>
       </c>
@@ -6424,7 +6468,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
         <v>193</v>
       </c>
@@ -6453,7 +6497,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>193</v>
       </c>
@@ -6482,7 +6526,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>193</v>
       </c>
@@ -6511,7 +6555,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
         <v>193</v>
       </c>
@@ -6540,7 +6584,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
         <v>193</v>
       </c>
@@ -6569,7 +6613,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>193</v>
       </c>
@@ -6598,7 +6642,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
         <v>193</v>
       </c>
@@ -6627,7 +6671,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
         <v>193</v>
       </c>
@@ -6656,7 +6700,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
         <v>193</v>
       </c>
@@ -6685,7 +6729,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12">
       <c r="A73" t="s">
         <v>193</v>
       </c>
@@ -6714,7 +6758,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12">
       <c r="A74" t="s">
         <v>193</v>
       </c>
@@ -6743,7 +6787,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12">
       <c r="A75" t="s">
         <v>193</v>
       </c>
@@ -6772,7 +6816,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12">
       <c r="A76" t="s">
         <v>193</v>
       </c>
@@ -6792,7 +6836,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12">
       <c r="A77" t="s">
         <v>193</v>
       </c>
@@ -6821,7 +6865,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12">
       <c r="A78" t="s">
         <v>193</v>
       </c>
@@ -6841,7 +6885,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12">
       <c r="A79" t="s">
         <v>193</v>
       </c>
@@ -6870,7 +6914,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12">
       <c r="A80" t="s">
         <v>193</v>
       </c>
@@ -6890,7 +6934,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12">
       <c r="A81" t="s">
         <v>193</v>
       </c>
@@ -6919,7 +6963,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12">
       <c r="A82" t="s">
         <v>193</v>
       </c>
@@ -6939,7 +6983,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12">
       <c r="A83" t="s">
         <v>193</v>
       </c>
@@ -6959,7 +7003,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12">
       <c r="A84" t="s">
         <v>193</v>
       </c>
@@ -6979,7 +7023,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12">
       <c r="A85" t="s">
         <v>193</v>
       </c>
@@ -6999,7 +7043,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12">
       <c r="A86" t="s">
         <v>193</v>
       </c>
@@ -7019,7 +7063,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12">
       <c r="A87" t="s">
         <v>193</v>
       </c>
@@ -7048,7 +7092,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12">
       <c r="A88" t="s">
         <v>193</v>
       </c>
@@ -7068,7 +7112,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12">
       <c r="A89" t="s">
         <v>193</v>
       </c>
@@ -7088,7 +7132,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12">
       <c r="A90" t="s">
         <v>193</v>
       </c>
@@ -7117,7 +7161,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12">
       <c r="A91" t="s">
         <v>193</v>
       </c>
@@ -7146,7 +7190,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12">
       <c r="A92" t="s">
         <v>193</v>
       </c>
@@ -7175,7 +7219,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12">
       <c r="A93" t="s">
         <v>193</v>
       </c>
@@ -7204,7 +7248,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12">
       <c r="A94" t="s">
         <v>193</v>
       </c>
@@ -7233,7 +7277,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12">
       <c r="A95" t="s">
         <v>193</v>
       </c>
@@ -7253,7 +7297,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12">
       <c r="A96" t="s">
         <v>193</v>
       </c>
@@ -7282,7 +7326,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12">
       <c r="A97" t="s">
         <v>193</v>
       </c>
@@ -7302,7 +7346,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12">
       <c r="A98" t="s">
         <v>193</v>
       </c>
@@ -7322,7 +7366,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12">
       <c r="A99" t="s">
         <v>193</v>
       </c>
@@ -7351,7 +7395,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12">
       <c r="A100" t="s">
         <v>193</v>
       </c>
@@ -7371,7 +7415,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12">
       <c r="A101" t="s">
         <v>193</v>
       </c>
@@ -7400,7 +7444,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12">
       <c r="A102" t="s">
         <v>193</v>
       </c>
@@ -7429,7 +7473,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12">
       <c r="A103" t="s">
         <v>193</v>
       </c>
@@ -7449,7 +7493,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12">
       <c r="A104" t="s">
         <v>193</v>
       </c>
@@ -7469,7 +7513,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12">
       <c r="A105" t="s">
         <v>193</v>
       </c>
@@ -7489,7 +7533,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12">
       <c r="A106" t="s">
         <v>193</v>
       </c>
@@ -7509,7 +7553,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:12">
       <c r="A107" t="s">
         <v>193</v>
       </c>
@@ -7529,7 +7573,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:12">
       <c r="A108" t="s">
         <v>193</v>
       </c>
@@ -7549,7 +7593,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:12">
       <c r="A109" t="s">
         <v>193</v>
       </c>
@@ -7569,7 +7613,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:12">
       <c r="A110" t="s">
         <v>193</v>
       </c>
@@ -7589,7 +7633,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:12">
       <c r="A111" t="s">
         <v>193</v>
       </c>
@@ -7609,7 +7653,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:12">
       <c r="A112" t="s">
         <v>193</v>
       </c>
@@ -7629,7 +7673,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12">
       <c r="A113" t="s">
         <v>193</v>
       </c>
@@ -7649,7 +7693,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12">
       <c r="A114" t="s">
         <v>193</v>
       </c>
@@ -7678,7 +7722,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12">
       <c r="A115" t="s">
         <v>193</v>
       </c>
@@ -7698,7 +7742,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12">
       <c r="A116" t="s">
         <v>193</v>
       </c>
@@ -7718,7 +7762,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12">
       <c r="A117" t="s">
         <v>193</v>
       </c>
@@ -7738,7 +7782,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12">
       <c r="A118" t="s">
         <v>193</v>
       </c>
@@ -7758,7 +7802,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12">
       <c r="A119" t="s">
         <v>652</v>
       </c>
@@ -7775,7 +7819,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12">
       <c r="A120" t="s">
         <v>652</v>
       </c>
@@ -7792,7 +7836,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12">
       <c r="A121" t="s">
         <v>652</v>
       </c>
@@ -7818,7 +7862,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12">
       <c r="A122" t="s">
         <v>652</v>
       </c>
@@ -7844,7 +7888,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12">
       <c r="A123" t="s">
         <v>652</v>
       </c>
@@ -7870,7 +7914,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12">
       <c r="A124" t="s">
         <v>652</v>
       </c>
@@ -7896,7 +7940,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12">
       <c r="A125" t="s">
         <v>652</v>
       </c>
@@ -7922,7 +7966,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12">
       <c r="A126" t="s">
         <v>652</v>
       </c>
@@ -7948,7 +7992,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12">
       <c r="A127" t="s">
         <v>652</v>
       </c>
@@ -7974,7 +8018,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12">
       <c r="A128" t="s">
         <v>652</v>
       </c>
@@ -8000,7 +8044,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:12">
       <c r="A129" t="s">
         <v>652</v>
       </c>
@@ -8026,7 +8070,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:12">
       <c r="A130" t="s">
         <v>652</v>
       </c>
@@ -8052,7 +8096,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:12">
       <c r="A131" t="s">
         <v>652</v>
       </c>
@@ -8078,7 +8122,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:12">
       <c r="A132" t="s">
         <v>652</v>
       </c>
@@ -8095,7 +8139,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:12">
       <c r="A133" t="s">
         <v>652</v>
       </c>
@@ -8121,7 +8165,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:12">
       <c r="A134" t="s">
         <v>652</v>
       </c>
@@ -8147,7 +8191,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:12">
       <c r="A135" t="s">
         <v>652</v>
       </c>
@@ -8173,7 +8217,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:12">
       <c r="A136" t="s">
         <v>652</v>
       </c>
@@ -8199,7 +8243,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:12">
       <c r="A137" t="s">
         <v>652</v>
       </c>
@@ -8216,7 +8260,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:12">
       <c r="A138" t="s">
         <v>652</v>
       </c>
@@ -8242,7 +8286,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:12">
       <c r="A139" t="s">
         <v>746</v>
       </c>
@@ -8256,7 +8300,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:12">
       <c r="A140" t="s">
         <v>746</v>
       </c>
@@ -8270,7 +8314,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:12">
       <c r="A141" t="s">
         <v>746</v>
       </c>
@@ -8284,7 +8328,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12">
       <c r="A142" t="s">
         <v>746</v>
       </c>
@@ -8298,7 +8342,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:12">
       <c r="A143" t="s">
         <v>746</v>
       </c>
@@ -8312,7 +8356,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:12">
       <c r="A144" t="s">
         <v>746</v>
       </c>
@@ -8326,7 +8370,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:12">
       <c r="A145" t="s">
         <v>746</v>
       </c>
@@ -8340,7 +8384,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:12">
       <c r="A146" t="s">
         <v>746</v>
       </c>
@@ -8354,7 +8398,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:12">
       <c r="A147" t="s">
         <v>746</v>
       </c>
@@ -8368,7 +8412,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:12">
       <c r="A148" t="s">
         <v>746</v>
       </c>
@@ -8382,7 +8426,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:12">
       <c r="A149" t="s">
         <v>746</v>
       </c>
@@ -8396,7 +8440,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12">
       <c r="A150" t="s">
         <v>746</v>
       </c>
@@ -8410,7 +8454,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:12">
       <c r="A151" t="s">
         <v>746</v>
       </c>
@@ -8424,7 +8468,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:12">
       <c r="A152" t="s">
         <v>746</v>
       </c>
@@ -8438,7 +8482,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:12">
       <c r="A153" t="s">
         <v>746</v>
       </c>
@@ -8452,7 +8496,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:12">
       <c r="A154" t="s">
         <v>746</v>
       </c>
@@ -8466,7 +8510,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:12">
       <c r="A155" t="s">
         <v>746</v>
       </c>
@@ -8480,7 +8524,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:12">
       <c r="A156" t="s">
         <v>746</v>
       </c>
@@ -8494,7 +8538,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:12">
       <c r="A157" t="s">
         <v>746</v>
       </c>
@@ -8508,7 +8552,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:12">
       <c r="A158" t="s">
         <v>746</v>
       </c>
@@ -8522,7 +8566,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:12">
       <c r="A159" t="s">
         <v>746</v>
       </c>
@@ -8536,7 +8580,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:12">
       <c r="A160" t="s">
         <v>746</v>
       </c>
@@ -8550,7 +8594,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:12">
       <c r="A161" t="s">
         <v>746</v>
       </c>
@@ -8564,7 +8608,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:12">
       <c r="A162" t="s">
         <v>746</v>
       </c>
@@ -8578,7 +8622,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:12">
       <c r="A163" t="s">
         <v>746</v>
       </c>
@@ -8592,7 +8636,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:12">
       <c r="A164" t="s">
         <v>746</v>
       </c>
@@ -8606,7 +8650,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:12">
       <c r="A165" t="s">
         <v>746</v>
       </c>
@@ -8620,7 +8664,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:12">
       <c r="A166" t="s">
         <v>746</v>
       </c>
@@ -8634,7 +8678,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:12">
       <c r="A167" t="s">
         <v>746</v>
       </c>
@@ -8648,7 +8692,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:12">
       <c r="A168" t="s">
         <v>746</v>
       </c>
@@ -8662,7 +8706,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:12">
       <c r="A169" t="s">
         <v>746</v>
       </c>
@@ -8676,7 +8720,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:12">
       <c r="A170" t="s">
         <v>746</v>
       </c>
@@ -8690,7 +8734,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:12">
       <c r="A171" t="s">
         <v>746</v>
       </c>
@@ -8704,7 +8748,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:12">
       <c r="A172" t="s">
         <v>746</v>
       </c>
@@ -8718,7 +8762,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:12">
       <c r="A173" t="s">
         <v>746</v>
       </c>
@@ -8732,7 +8776,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:12">
       <c r="A174" t="s">
         <v>746</v>
       </c>
@@ -8746,7 +8790,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:12">
       <c r="A175" t="s">
         <v>746</v>
       </c>
@@ -8760,7 +8804,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:12">
       <c r="A176" t="s">
         <v>746</v>
       </c>
@@ -8774,7 +8818,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:12">
       <c r="A177" t="s">
         <v>746</v>
       </c>
@@ -8788,7 +8832,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:12">
       <c r="A178" t="s">
         <v>746</v>
       </c>
@@ -8802,7 +8846,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:12">
       <c r="A179" t="s">
         <v>746</v>
       </c>
@@ -8816,7 +8860,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:12">
       <c r="A180" t="s">
         <v>746</v>
       </c>
@@ -8830,7 +8874,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:12">
       <c r="A181" t="s">
         <v>746</v>
       </c>
@@ -8844,7 +8888,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:12">
       <c r="A182" t="s">
         <v>746</v>
       </c>
@@ -8858,7 +8902,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:12">
       <c r="A183" t="s">
         <v>746</v>
       </c>
@@ -8872,7 +8916,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:12">
       <c r="A184" t="s">
         <v>746</v>
       </c>
@@ -8886,7 +8930,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:12">
       <c r="A185" t="s">
         <v>746</v>
       </c>
@@ -8900,7 +8944,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:12">
       <c r="A186" t="s">
         <v>746</v>
       </c>
@@ -8914,7 +8958,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:12">
       <c r="A187" t="s">
         <v>746</v>
       </c>
@@ -8928,7 +8972,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:12">
       <c r="A188" t="s">
         <v>746</v>
       </c>
@@ -8942,7 +8986,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:12">
       <c r="A189" t="s">
         <v>746</v>
       </c>
@@ -8956,7 +9000,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:12">
       <c r="A190" t="s">
         <v>746</v>
       </c>
@@ -8970,7 +9014,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:12">
       <c r="A191" t="s">
         <v>746</v>
       </c>
@@ -8984,7 +9028,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:12">
       <c r="A192" t="s">
         <v>746</v>
       </c>
@@ -8998,7 +9042,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:12">
       <c r="A193" t="s">
         <v>746</v>
       </c>
@@ -9012,7 +9056,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:12">
       <c r="A194" t="s">
         <v>746</v>
       </c>
@@ -9026,7 +9070,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:12">
       <c r="A195" t="s">
         <v>746</v>
       </c>
@@ -9040,7 +9084,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:12">
       <c r="A196" t="s">
         <v>746</v>
       </c>
@@ -9054,7 +9098,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:12">
       <c r="A197" t="s">
         <v>746</v>
       </c>
@@ -9068,7 +9112,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:12">
       <c r="A198" t="s">
         <v>746</v>
       </c>
@@ -9082,7 +9126,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:12">
       <c r="A199" t="s">
         <v>746</v>
       </c>
@@ -9096,7 +9140,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:12">
       <c r="A200" t="s">
         <v>746</v>
       </c>
@@ -9110,7 +9154,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:12">
       <c r="A201" t="s">
         <v>746</v>
       </c>
@@ -9124,7 +9168,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:12">
       <c r="A202" t="s">
         <v>746</v>
       </c>
@@ -9138,7 +9182,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:12">
       <c r="A203" t="s">
         <v>746</v>
       </c>
@@ -9152,7 +9196,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:12">
       <c r="A204" t="s">
         <v>746</v>
       </c>
@@ -9166,7 +9210,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:12">
       <c r="A205" t="s">
         <v>746</v>
       </c>
@@ -9180,7 +9224,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:12">
       <c r="A206" t="s">
         <v>746</v>
       </c>
@@ -9194,7 +9238,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:12">
       <c r="A207" t="s">
         <v>746</v>
       </c>
@@ -9208,7 +9252,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:12">
       <c r="A208" t="s">
         <v>746</v>
       </c>
@@ -9222,7 +9266,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:12">
       <c r="A209" t="s">
         <v>746</v>
       </c>
@@ -9236,7 +9280,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:12">
       <c r="A210" t="s">
         <v>746</v>
       </c>
@@ -9250,7 +9294,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:12">
       <c r="A211" t="s">
         <v>746</v>
       </c>
@@ -9264,7 +9308,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:12">
       <c r="A212" t="s">
         <v>746</v>
       </c>
@@ -9278,7 +9322,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:12">
       <c r="A213" t="s">
         <v>746</v>
       </c>
@@ -9292,7 +9336,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:12">
       <c r="A214" t="s">
         <v>746</v>
       </c>
@@ -9306,7 +9350,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:12">
       <c r="A215" t="s">
         <v>746</v>
       </c>
@@ -9320,7 +9364,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:12">
       <c r="A216" t="s">
         <v>746</v>
       </c>
@@ -9334,7 +9378,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:12">
       <c r="A217" t="s">
         <v>746</v>
       </c>
@@ -9348,7 +9392,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:12">
       <c r="A218" t="s">
         <v>746</v>
       </c>
@@ -9362,7 +9406,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:12">
       <c r="A219" t="s">
         <v>746</v>
       </c>
@@ -9376,7 +9420,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:12">
       <c r="A220" t="s">
         <v>746</v>
       </c>
@@ -9390,7 +9434,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:12">
       <c r="A221" t="s">
         <v>746</v>
       </c>
@@ -9404,7 +9448,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:12">
       <c r="A222" t="s">
         <v>746</v>
       </c>
@@ -9418,7 +9462,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:12">
       <c r="A223" t="s">
         <v>746</v>
       </c>
@@ -9432,7 +9476,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:12">
       <c r="A224" t="s">
         <v>746</v>
       </c>
@@ -9446,7 +9490,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:12">
       <c r="A225" t="s">
         <v>746</v>
       </c>
@@ -9460,7 +9504,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:12">
       <c r="A226" t="s">
         <v>746</v>
       </c>
@@ -9474,7 +9518,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:12">
       <c r="A227" t="s">
         <v>746</v>
       </c>
@@ -9488,7 +9532,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:12">
       <c r="A228" t="s">
         <v>746</v>
       </c>
@@ -9502,7 +9546,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:12">
       <c r="A229" t="s">
         <v>746</v>
       </c>
@@ -9516,7 +9560,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:12">
       <c r="A230" t="s">
         <v>746</v>
       </c>
@@ -9530,7 +9574,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:12">
       <c r="A231" t="s">
         <v>746</v>
       </c>
@@ -9544,7 +9588,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:12">
       <c r="A232" t="s">
         <v>746</v>
       </c>
@@ -9558,7 +9602,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:12">
       <c r="A233" t="s">
         <v>746</v>
       </c>
@@ -9572,7 +9616,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:12">
       <c r="A234" t="s">
         <v>746</v>
       </c>
@@ -9586,7 +9630,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:12">
       <c r="A235" t="s">
         <v>746</v>
       </c>
@@ -9600,7 +9644,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:12">
       <c r="A236" t="s">
         <v>746</v>
       </c>
@@ -9614,7 +9658,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:12">
       <c r="A237" t="s">
         <v>746</v>
       </c>
@@ -9628,7 +9672,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:12">
       <c r="A238" t="s">
         <v>746</v>
       </c>
@@ -9642,7 +9686,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:12">
       <c r="A239" t="s">
         <v>746</v>
       </c>
@@ -9656,7 +9700,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:12">
       <c r="A240" t="s">
         <v>746</v>
       </c>
@@ -9670,7 +9714,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:12">
       <c r="A241" t="s">
         <v>746</v>
       </c>
@@ -9684,7 +9728,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:12">
       <c r="A242" t="s">
         <v>746</v>
       </c>
@@ -9698,7 +9742,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:12">
       <c r="A243" t="s">
         <v>746</v>
       </c>
@@ -9712,7 +9756,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:12">
       <c r="A244" t="s">
         <v>746</v>
       </c>
@@ -9726,7 +9770,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:12">
       <c r="A245" t="s">
         <v>746</v>
       </c>
@@ -9740,7 +9784,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:12">
       <c r="A246" t="s">
         <v>746</v>
       </c>
@@ -9754,7 +9798,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:12">
       <c r="A247" t="s">
         <v>746</v>
       </c>
@@ -9768,7 +9812,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:12">
       <c r="A248" t="s">
         <v>746</v>
       </c>
@@ -9782,7 +9826,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:12">
       <c r="A249" t="s">
         <v>746</v>
       </c>
@@ -9796,7 +9840,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:12">
       <c r="A250" t="s">
         <v>746</v>
       </c>
@@ -9810,7 +9854,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:12">
       <c r="A251" t="s">
         <v>746</v>
       </c>
@@ -9824,7 +9868,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:12">
       <c r="A252" t="s">
         <v>746</v>
       </c>
@@ -9838,7 +9882,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:12">
       <c r="A253" t="s">
         <v>746</v>
       </c>
@@ -9852,7 +9896,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:12">
       <c r="A254" t="s">
         <v>746</v>
       </c>
@@ -9866,7 +9910,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:12">
       <c r="A255" t="s">
         <v>746</v>
       </c>
@@ -9880,7 +9924,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:12">
       <c r="A256" t="s">
         <v>746</v>
       </c>
@@ -9894,7 +9938,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:12">
       <c r="A257" t="s">
         <v>746</v>
       </c>
@@ -9908,7 +9952,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:12">
       <c r="A258" t="s">
         <v>746</v>
       </c>
@@ -9922,7 +9966,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:12">
       <c r="A259" t="s">
         <v>746</v>
       </c>
@@ -9936,7 +9980,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:12">
       <c r="A260" t="s">
         <v>746</v>
       </c>
@@ -9950,7 +9994,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:12">
       <c r="A261" t="s">
         <v>746</v>
       </c>
@@ -9964,7 +10008,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:12">
       <c r="A262" t="s">
         <v>746</v>
       </c>
@@ -9978,7 +10022,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:12">
       <c r="A263" t="s">
         <v>746</v>
       </c>
@@ -9992,7 +10036,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:12">
       <c r="A264" t="s">
         <v>746</v>
       </c>
@@ -10006,7 +10050,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:12">
       <c r="A265" t="s">
         <v>746</v>
       </c>
@@ -10020,7 +10064,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:12">
       <c r="A266" t="s">
         <v>746</v>
       </c>
@@ -10034,7 +10078,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:12">
       <c r="A267" t="s">
         <v>746</v>
       </c>
@@ -10048,7 +10092,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:12">
       <c r="A268" t="s">
         <v>746</v>
       </c>
@@ -10062,7 +10106,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:12">
       <c r="A269" t="s">
         <v>746</v>
       </c>
@@ -10076,7 +10120,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:12">
       <c r="A270" t="s">
         <v>746</v>
       </c>
@@ -10090,7 +10134,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:12">
       <c r="A271" t="s">
         <v>746</v>
       </c>
@@ -10104,7 +10148,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:12">
       <c r="A272" t="s">
         <v>746</v>
       </c>
@@ -10118,7 +10162,7 @@
         <v>1133</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:12">
       <c r="A273" t="s">
         <v>746</v>
       </c>
@@ -10132,7 +10176,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:12">
       <c r="A274" t="s">
         <v>746</v>
       </c>
@@ -10146,7 +10190,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:12">
       <c r="A275" t="s">
         <v>746</v>
       </c>
@@ -10160,7 +10204,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:12">
       <c r="A276" t="s">
         <v>746</v>
       </c>
@@ -10174,7 +10218,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:12">
       <c r="A277" t="s">
         <v>746</v>
       </c>
@@ -10188,7 +10232,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:12">
       <c r="A278" t="s">
         <v>746</v>
       </c>
@@ -10202,7 +10246,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:12">
       <c r="A279" t="s">
         <v>746</v>
       </c>
@@ -10216,7 +10260,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:12">
       <c r="A280" t="s">
         <v>746</v>
       </c>
@@ -10230,7 +10274,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:12">
       <c r="A281" t="s">
         <v>746</v>
       </c>
@@ -10244,7 +10288,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:12">
       <c r="A282" t="s">
         <v>746</v>
       </c>
@@ -10258,7 +10302,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:12">
       <c r="A283" t="s">
         <v>746</v>
       </c>
@@ -10272,7 +10316,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:12">
       <c r="A284" t="s">
         <v>746</v>
       </c>
@@ -10286,7 +10330,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:12">
       <c r="A285" t="s">
         <v>746</v>
       </c>
@@ -10300,7 +10344,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:12">
       <c r="A286" t="s">
         <v>746</v>
       </c>
@@ -10314,7 +10358,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:12">
       <c r="A287" t="s">
         <v>746</v>
       </c>
@@ -10328,7 +10372,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:12">
       <c r="A288" t="s">
         <v>746</v>
       </c>
@@ -10342,7 +10386,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:12">
       <c r="A289" t="s">
         <v>746</v>
       </c>
@@ -10356,7 +10400,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:12">
       <c r="A290" t="s">
         <v>746</v>
       </c>
@@ -10370,7 +10414,7 @@
         <v>1174</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:12">
       <c r="A291" t="s">
         <v>746</v>
       </c>
@@ -10384,7 +10428,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:12">
       <c r="A292" t="s">
         <v>746</v>
       </c>
@@ -10398,7 +10442,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:12">
       <c r="A293" t="s">
         <v>746</v>
       </c>
@@ -10412,7 +10456,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:12">
       <c r="A294" t="s">
         <v>746</v>
       </c>
@@ -10426,7 +10470,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:12">
       <c r="A295" t="s">
         <v>746</v>
       </c>
@@ -10440,7 +10484,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:12">
       <c r="A296" t="s">
         <v>746</v>
       </c>
@@ -10454,7 +10498,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:12">
       <c r="A297" t="s">
         <v>746</v>
       </c>
@@ -10468,7 +10512,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:12">
       <c r="A298" t="s">
         <v>746</v>
       </c>
@@ -10482,7 +10526,7 @@
         <v>1193</v>
       </c>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:12">
       <c r="A299" t="s">
         <v>746</v>
       </c>
@@ -10496,7 +10540,7 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:12">
       <c r="A300" t="s">
         <v>746</v>
       </c>
@@ -10510,7 +10554,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:12">
       <c r="A301" t="s">
         <v>746</v>
       </c>
@@ -10524,7 +10568,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:12">
       <c r="A302" t="s">
         <v>746</v>
       </c>
@@ -10538,7 +10582,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:12">
       <c r="A303" t="s">
         <v>746</v>
       </c>
@@ -10552,7 +10596,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:12">
       <c r="A304" t="s">
         <v>746</v>
       </c>
@@ -10566,7 +10610,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:12">
       <c r="A305" t="s">
         <v>746</v>
       </c>
@@ -10580,7 +10624,7 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:12">
       <c r="A306" t="s">
         <v>746</v>
       </c>
@@ -10594,7 +10638,7 @@
         <v>1214</v>
       </c>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:12">
       <c r="A307" t="s">
         <v>746</v>
       </c>
@@ -10608,7 +10652,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:12">
       <c r="A308" t="s">
         <v>746</v>
       </c>
@@ -10622,7 +10666,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:12">
       <c r="A309" t="s">
         <v>746</v>
       </c>
@@ -10636,7 +10680,7 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:12">
       <c r="A310" t="s">
         <v>746</v>
       </c>
@@ -10650,7 +10694,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:12">
       <c r="A311" t="s">
         <v>746</v>
       </c>
@@ -10664,7 +10708,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:12">
       <c r="A312" t="s">
         <v>746</v>
       </c>
@@ -10678,7 +10722,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:12">
       <c r="A313" t="s">
         <v>746</v>
       </c>
@@ -10692,7 +10736,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:12">
       <c r="A314" t="s">
         <v>746</v>
       </c>
@@ -10706,7 +10750,7 @@
         <v>1232</v>
       </c>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:12">
       <c r="A315" t="s">
         <v>746</v>
       </c>
@@ -10720,7 +10764,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:12">
       <c r="A316" t="s">
         <v>746</v>
       </c>
@@ -10734,7 +10778,7 @@
         <v>1237</v>
       </c>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:12">
       <c r="A317" t="s">
         <v>746</v>
       </c>
@@ -10748,7 +10792,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:12">
       <c r="A318" t="s">
         <v>746</v>
       </c>
@@ -10762,7 +10806,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:12">
       <c r="A319" t="s">
         <v>746</v>
       </c>
@@ -10776,7 +10820,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:12">
       <c r="A320" t="s">
         <v>746</v>
       </c>
@@ -10790,7 +10834,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:12">
       <c r="A321" t="s">
         <v>746</v>
       </c>
@@ -10804,7 +10848,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:12">
       <c r="A322" t="s">
         <v>746</v>
       </c>
@@ -10818,7 +10862,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:12">
       <c r="A323" t="s">
         <v>746</v>
       </c>
@@ -10832,7 +10876,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:12">
       <c r="A324" t="s">
         <v>746</v>
       </c>
@@ -10846,7 +10890,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:12">
       <c r="A325" t="s">
         <v>746</v>
       </c>
@@ -10860,7 +10904,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:12">
       <c r="A326" t="s">
         <v>746</v>
       </c>
@@ -10874,7 +10918,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:12">
       <c r="A327" t="s">
         <v>746</v>
       </c>
@@ -10888,7 +10932,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:12">
       <c r="A328" t="s">
         <v>746</v>
       </c>
@@ -10902,7 +10946,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:12">
       <c r="A329" t="s">
         <v>746</v>
       </c>
@@ -10916,7 +10960,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="330" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:12">
       <c r="A330" t="s">
         <v>746</v>
       </c>
@@ -10930,7 +10974,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="331" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:12">
       <c r="A331" t="s">
         <v>746</v>
       </c>
@@ -10944,7 +10988,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:12">
       <c r="A332" t="s">
         <v>746</v>
       </c>
@@ -10958,7 +11002,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="333" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:12">
       <c r="A333" t="s">
         <v>746</v>
       </c>
@@ -10972,7 +11016,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="334" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:12">
       <c r="A334" t="s">
         <v>746</v>
       </c>
@@ -10986,7 +11030,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="335" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:12">
       <c r="A335" t="s">
         <v>746</v>
       </c>
@@ -11000,7 +11044,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="336" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:12">
       <c r="A336" t="s">
         <v>746</v>
       </c>
@@ -11014,7 +11058,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="337" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:12">
       <c r="A337" t="s">
         <v>746</v>
       </c>
@@ -11028,7 +11072,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="338" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:12">
       <c r="A338" t="s">
         <v>746</v>
       </c>
@@ -11042,7 +11086,7 @@
         <v>1282</v>
       </c>
     </row>
-    <row r="339" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:12">
       <c r="A339" t="s">
         <v>746</v>
       </c>
@@ -11056,7 +11100,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="340" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:12">
       <c r="A340" t="s">
         <v>746</v>
       </c>
@@ -11070,7 +11114,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="341" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:12">
       <c r="A341" t="s">
         <v>746</v>
       </c>
@@ -11084,7 +11128,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="342" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:12">
       <c r="A342" t="s">
         <v>746</v>
       </c>
@@ -11098,7 +11142,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="343" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:12">
       <c r="A343" t="s">
         <v>746</v>
       </c>
@@ -11112,7 +11156,7 @@
         <v>1294</v>
       </c>
     </row>
-    <row r="344" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:12">
       <c r="A344" t="s">
         <v>746</v>
       </c>
@@ -11126,7 +11170,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="345" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:12">
       <c r="A345" t="s">
         <v>746</v>
       </c>
@@ -11140,7 +11184,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="346" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:12">
       <c r="A346" t="s">
         <v>746</v>
       </c>
@@ -11154,7 +11198,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="347" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:12">
       <c r="A347" t="s">
         <v>746</v>
       </c>
@@ -11168,7 +11212,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="348" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:12">
       <c r="A348" t="s">
         <v>746</v>
       </c>
@@ -11182,7 +11226,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="349" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:12">
       <c r="A349" t="s">
         <v>746</v>
       </c>
@@ -11196,7 +11240,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="350" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:12">
       <c r="A350" t="s">
         <v>746</v>
       </c>
@@ -11210,7 +11254,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="351" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:12">
       <c r="A351" t="s">
         <v>746</v>
       </c>
@@ -11224,7 +11268,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="352" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:12">
       <c r="A352" t="s">
         <v>746</v>
       </c>
@@ -11238,7 +11282,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="353" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:12">
       <c r="A353" t="s">
         <v>746</v>
       </c>
@@ -11252,7 +11296,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="354" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:12">
       <c r="A354" t="s">
         <v>746</v>
       </c>
@@ -11266,7 +11310,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="355" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:12">
       <c r="A355" t="s">
         <v>746</v>
       </c>
@@ -11280,7 +11324,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="356" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:12">
       <c r="A356" t="s">
         <v>1323</v>
       </c>
@@ -11297,7 +11341,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="357" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:12">
       <c r="A357" t="s">
         <v>1323</v>
       </c>
@@ -11314,7 +11358,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="358" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:12">
       <c r="A358" t="s">
         <v>1323</v>
       </c>
@@ -11331,7 +11375,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="359" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:12">
       <c r="A359" t="s">
         <v>1323</v>
       </c>
@@ -11348,7 +11392,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="360" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:12">
       <c r="A360" t="s">
         <v>1336</v>
       </c>
@@ -11365,7 +11409,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="361" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:12">
       <c r="A361" t="s">
         <v>1323</v>
       </c>
@@ -11382,7 +11426,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="362" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:12">
       <c r="A362" t="s">
         <v>1323</v>
       </c>
@@ -11399,7 +11443,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="363" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:12">
       <c r="A363" t="s">
         <v>1346</v>
       </c>
@@ -11413,7 +11457,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="364" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:12">
       <c r="A364" t="s">
         <v>1350</v>
       </c>
@@ -11430,7 +11474,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="365" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:12">
       <c r="A365" t="s">
         <v>1323</v>
       </c>
@@ -11447,7 +11491,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="366" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:12">
       <c r="A366" t="s">
         <v>1323</v>
       </c>
@@ -11464,7 +11508,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="367" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:12">
       <c r="A367" t="s">
         <v>1360</v>
       </c>
@@ -11481,7 +11525,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="368" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:12">
       <c r="A368" t="s">
         <v>1323</v>
       </c>
@@ -11498,7 +11542,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="369" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:12">
       <c r="A369" t="s">
         <v>1336</v>
       </c>
@@ -11515,7 +11559,7 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="370" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:12">
       <c r="A370" t="s">
         <v>1336</v>
       </c>
@@ -11532,7 +11576,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="371" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:12">
       <c r="A371" t="s">
         <v>1336</v>
       </c>
@@ -11549,7 +11593,7 @@
         <v>1375</v>
       </c>
     </row>
-    <row r="372" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:12">
       <c r="A372" t="s">
         <v>1336</v>
       </c>
@@ -11566,7 +11610,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="373" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:12">
       <c r="A373" t="s">
         <v>1336</v>
       </c>
@@ -11583,7 +11627,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="374" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:12">
       <c r="A374" t="s">
         <v>1336</v>
       </c>
@@ -11600,7 +11644,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="375" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:12">
       <c r="A375" t="s">
         <v>1336</v>
       </c>
@@ -11617,7 +11661,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="376" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:12">
       <c r="A376" t="s">
         <v>1336</v>
       </c>
@@ -11634,7 +11678,7 @@
         <v>1388</v>
       </c>
     </row>
-    <row r="377" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:12">
       <c r="A377" t="s">
         <v>1323</v>
       </c>
@@ -11651,7 +11695,7 @@
         <v>1391</v>
       </c>
     </row>
-    <row r="378" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:12">
       <c r="A378" t="s">
         <v>1323</v>
       </c>
@@ -11668,7 +11712,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="379" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:12">
       <c r="A379" t="s">
         <v>1323</v>
       </c>
@@ -11685,7 +11729,7 @@
         <v>1397</v>
       </c>
     </row>
-    <row r="380" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:12">
       <c r="A380" t="s">
         <v>1323</v>
       </c>
@@ -11702,7 +11746,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="381" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:12">
       <c r="A381" t="s">
         <v>1323</v>
       </c>
@@ -11719,7 +11763,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="382" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:12">
       <c r="A382" t="s">
         <v>1336</v>
       </c>
@@ -11736,7 +11780,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="383" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:12">
       <c r="A383" t="s">
         <v>1336</v>
       </c>
@@ -11753,7 +11797,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="384" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:12">
       <c r="A384" t="s">
         <v>1323</v>
       </c>
@@ -11768,6 +11812,57 @@
       </c>
       <c r="L384" t="s">
         <v>1412</v>
+      </c>
+    </row>
+    <row r="385" spans="1:12">
+      <c r="A385" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B385" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C385" t="s">
+        <v>1413</v>
+      </c>
+      <c r="D385" t="s">
+        <v>1417</v>
+      </c>
+      <c r="G385" t="s">
+        <v>87</v>
+      </c>
+      <c r="L385" s="3" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="386" spans="1:12">
+      <c r="A386" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B386" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C386" t="s">
+        <v>1418</v>
+      </c>
+      <c r="G386" t="s">
+        <v>1420</v>
+      </c>
+      <c r="L386" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="387" spans="1:12">
+      <c r="A387" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C387" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="G387" t="s">
+        <v>1210</v>
+      </c>
+      <c r="L387" t="s">
+        <v>1424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small changes in polymerase tsv
</commit_message>
<xml_diff>
--- a/data/combined_polymerases.xlsx
+++ b/data/combined_polymerases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idamei/wzy_polymerases/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4C2DC8-2ED9-B347-8654-B83FEFD42B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9730C4BD-8EFE-3240-967E-AE6B28F61C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2360" windowWidth="30240" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1900" uniqueCount="1425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="1442">
   <si>
     <t>species</t>
   </si>
@@ -3532,9 +3532,6 @@
     <t>AJ426045</t>
   </si>
   <si>
-    <t>MKVKAVPAITFYLSLMLTILVLLFGNEPNKSQYILVIATITVFYIAYITNKITSPASLLVISSFVFLGCRPLLSLFANYDYRIADWFIEGYMDDDVILANYAITLMYYGYTLGLILCKNTEKFYPHGPYPEKQLLKIKFLLTLFFLGSIGMVVKGIFFFNFIESNSYVDIYQSNITTPIGYDFLSYLFYCSFFLICAFHIQFRTNKKFLFIAICIAAFSTLKGSRSEAITFLLTVTCIYFNEVKTRNLRLLITMIFVFSVIFVISEFISMWRTGGSFFQLMQGNNPVINFVYGMGVSYLSIYQSVKLQLLSGGYNVTYLFSQLIITCSIFNVKLSLPEISYSHLASYTANPELYNLGFGLGGSYLAESFLAFGLIGCFIIPFLLLLNLNVLEKYTKNKPIIYFVYYSVLPPILFTPRETLFYFFPYLVKSIFVAFLVTLYIQYKKD</t>
-  </si>
-  <si>
     <t>CP002185</t>
   </si>
   <si>
@@ -3979,9 +3976,6 @@
     <t>AB627352</t>
   </si>
   <si>
-    <t>O183√Ç</t>
-  </si>
-  <si>
     <t>MIIITSFMVLLFLFTDNLKLKNFRIILFYFFSLCFSVLVYFRPEYMLNTDYKEYYNYFKWINFDNIYNLSDAIGFEYGFGYIVTLLKYFFESERACFSGIAFLSVFISYKAILRLNPKTTAFSFSLFLLSFCVYIFLGQIRQGISLSLGLLAISYLLEDKRKQFLLTVIIASSIHVTALILILAPFVKYFRIKYIFYSLLLSFAFVFIDVIKPLIITLAQFIPFGSFITGKIIAYGNSEFSTKVGFSFIQVYYVLLSTVLYILVKKYEYKNNYILILCKIFMVGVILNFTFNSFSVLLRITYYYLALDCILLGYLLNMAKNGYTKILIYCPTLMLFILRFYMQWSEHING</t>
   </si>
   <si>
@@ -4295,13 +4289,70 @@
   </si>
   <si>
     <t>MTYFTGFILILFAIIIKRLTPSQSKKNIVLIANAFWGILLVGYAFNEQYFVPLSATTLFFILAFLFFFSMTYILIARSGRVVFSFGTGFIESKYIYWFAGMINIISICFGIILLYNNHFSLKVMREGILDGSISGFGLGISLPLSFCCMYLARHENKKNYFYCFTLLSFLLAVLSTSKIFLILFLVYIVGINSYVSKKKLLIYGVFVFGLFALSSIILGKFSSDPEGKIISAIFDTLRVYLFSGLAAFNLYVEKNATLPENLLLYPFKEVWGTTKDIPKTDILPWINIGVWDTNVYTAFAPWYQSLGLYAAIIIGILLGFYYGIWFSFRQNLAVGFYQTFLCFPLLMLFFQEHYLLSWKMHFIYFLCAILLAMRKALEYE</t>
+  </si>
+  <si>
+    <t>pubmed</t>
+  </si>
+  <si>
+    <t>experimentally_characterized</t>
+  </si>
+  <si>
+    <t>AAA97573.1</t>
+  </si>
+  <si>
+    <t>U26685.1</t>
+  </si>
+  <si>
+    <t>MYILARVDRSILLNTVLLFAFFSATVWVNNNYIYHLYDYMGSAKKTVDFGLYPYLMVLALICALLCGGAIRSPGDLLVTLLVVILVPHSLVLNGANQYSPDAQPWAGVPLAIAFGILIIGIVNKIRFHPLGALQRENQGRRMLVLLSVLNIVVLVFIFFKSAGYFSFDFAGQYARRALAREVFAAGSANGYLSSIGTQAFFPVLFAWGVYRRQWFYLVLGIVNALVLWGAFGQKYPFVVLFLIYGLMVYFRRFGQVRVSWVVCALLMLLLLGALEHEVFGYSFLNDYFLRRAFIVPSTLLGAVDQFVSQFGSNYYRDTLLGALLGQGRTEPLSFRLGTEIFNNPDMNANVNFFAIAYMQLGYVGVMAESMLVGGSVVLMNFLFSRYGAFMAIPVALLFTTKILEQSLLTVMLGSGVFLMLLFLALISFPLKMSLGKTL</t>
+  </si>
+  <si>
+    <t>U50396.1</t>
+  </si>
+  <si>
+    <t>AAC45857.1</t>
+  </si>
+  <si>
+    <t>MYILARVDRSILLNTVLLFAFFSATVWVNNNYIYHLYDYMGSAKKTVDFGLYPYLMVLALICALLCGGAIRRPGDLLVTLLVVILVPHSLVLNGANQYSPDAQPWAGVPLAIAFGILIIGIVNKIRFHPLGALQRENQGRRMLVLLSVLNIVVLVFIFFKSAGYFSFDFAGQYARRALAREVFAAGSANGYLSSIGTQAFFPVLFAWGVYRRQWFYLVLGIVNALVLWGAFGQKYPFVVLFLIYGLMVYFRRFGQVRVSWVVCALLMLLLLGALEHEVFGYSFLNDYFLRRAFIVPSTLLGAVDQFVSQFGSNYYRDTLLGALLGQGRTEPLSFRLGTEIFNNPDMNANVNFFAIAYMQLGYVGVMAESMLVGGSVVLMNFLFSRYGAFMAIPVALLFTTKILEQPLLTVMLGSGVFLILLFLALISFPLKMSLGKTL</t>
+  </si>
+  <si>
+    <t>WP_001300154</t>
+  </si>
+  <si>
+    <t>WP_074526664.1</t>
+  </si>
+  <si>
+    <t>WP_038349068.1</t>
+  </si>
+  <si>
+    <t>WP_024244058.1</t>
+  </si>
+  <si>
+    <t>WP_046788607.1</t>
+  </si>
+  <si>
+    <t>WP_000456161.1</t>
+  </si>
+  <si>
+    <t>WP_000549530.1</t>
+  </si>
+  <si>
+    <t>O183</t>
+  </si>
+  <si>
+    <t>WP_052920558.1</t>
+  </si>
+  <si>
+    <t>WP_000864940</t>
+  </si>
+  <si>
+    <t>MKVKAVPAITFYLSLMLTILVLLFGNEPNKSQYILVIATITVFYIAYITNKITSPASLLVISSFVFLGCRPLLSLFANYDYRIADWFIEGYMDDDVILANYAITLMYYGYTLGLILCKNTEKFYPHGPYPEKQLLKIKFLLTLFFLGSIGMVVKGIFFFNFIESNSYVDIYQSNITTPIGYDFLSYLFYCSFFLICAFHIQFRTNKKFLFIAICIAAFSTLKGSRSEAITFLLTVTCIYFNEVKTRNLRLLITMIFVFSVIFVISEFISMWRTGGSFFQLMQGNNPVINFVYGMGVSYLSIYQSVKLQLLSGGYNVTYLFSQLIITCSSIFNVKLSLPEISYSHLASYTANPELYNLGFGLGGSYLAESFLAFGLIGCFIIPFLLLLNLNVLEKYTKNKPIIYFVYYSVLPPILFTPRESLFYFFPYLVKSIFVAFLVTLYIQYKKD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4326,6 +4377,32 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFA9B7C6"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4335,7 +4412,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -4358,11 +4435,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4370,8 +4459,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4672,15 +4774,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L387"/>
+  <dimension ref="A1:N389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A367" workbookViewId="0">
-      <selection activeCell="H389" sqref="H389"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="D139" sqref="D139:D344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4693,7 +4795,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -4714,11 +4816,17 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="5" t="s">
+        <v>1423</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4750,7 +4858,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -4785,7 +4893,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -4808,7 +4916,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -4831,7 +4939,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4866,7 +4974,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -4889,7 +4997,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -4921,7 +5029,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -4944,7 +5052,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -4976,7 +5084,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -5011,7 +5119,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -5046,7 +5154,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -5078,7 +5186,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -5101,7 +5209,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -5124,7 +5232,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -10372,9 +10480,12 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="288" spans="1:12">
+    <row r="288" spans="1:12" ht="16">
       <c r="A288" t="s">
         <v>746</v>
+      </c>
+      <c r="C288" s="6" t="s">
+        <v>1440</v>
       </c>
       <c r="E288" t="s">
         <v>1169</v>
@@ -10382,8 +10493,8 @@
       <c r="G288" t="s">
         <v>53</v>
       </c>
-      <c r="L288" t="s">
-        <v>1170</v>
+      <c r="L288" s="9" t="s">
+        <v>1441</v>
       </c>
     </row>
     <row r="289" spans="1:12">
@@ -10391,13 +10502,13 @@
         <v>746</v>
       </c>
       <c r="E289" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="G289" t="s">
         <v>53</v>
       </c>
       <c r="L289" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="290" spans="1:12">
@@ -10405,13 +10516,13 @@
         <v>746</v>
       </c>
       <c r="E290" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="G290" t="s">
         <v>59</v>
       </c>
       <c r="L290" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="291" spans="1:12">
@@ -10419,13 +10530,13 @@
         <v>746</v>
       </c>
       <c r="E291" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="G291" t="s">
         <v>59</v>
       </c>
       <c r="L291" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="292" spans="1:12">
@@ -10433,13 +10544,13 @@
         <v>746</v>
       </c>
       <c r="E292" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="G292" t="s">
         <v>59</v>
       </c>
       <c r="L292" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="293" spans="1:12">
@@ -10447,13 +10558,13 @@
         <v>746</v>
       </c>
       <c r="E293" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="G293" t="s">
         <v>66</v>
       </c>
       <c r="L293" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="294" spans="1:12">
@@ -10461,13 +10572,13 @@
         <v>746</v>
       </c>
       <c r="E294" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="G294" t="s">
         <v>79</v>
       </c>
       <c r="L294" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="295" spans="1:12">
@@ -10475,13 +10586,13 @@
         <v>746</v>
       </c>
       <c r="E295" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G295" t="s">
         <v>1183</v>
       </c>
-      <c r="G295" t="s">
+      <c r="L295" t="s">
         <v>1184</v>
-      </c>
-      <c r="L295" t="s">
-        <v>1185</v>
       </c>
     </row>
     <row r="296" spans="1:12">
@@ -10489,13 +10600,13 @@
         <v>746</v>
       </c>
       <c r="E296" t="s">
+        <v>1185</v>
+      </c>
+      <c r="G296" t="s">
         <v>1186</v>
       </c>
-      <c r="G296" t="s">
+      <c r="L296" t="s">
         <v>1187</v>
-      </c>
-      <c r="L296" t="s">
-        <v>1188</v>
       </c>
     </row>
     <row r="297" spans="1:12">
@@ -10503,13 +10614,13 @@
         <v>746</v>
       </c>
       <c r="E297" t="s">
+        <v>1188</v>
+      </c>
+      <c r="G297" t="s">
+        <v>1186</v>
+      </c>
+      <c r="L297" t="s">
         <v>1189</v>
-      </c>
-      <c r="G297" t="s">
-        <v>1187</v>
-      </c>
-      <c r="L297" t="s">
-        <v>1190</v>
       </c>
     </row>
     <row r="298" spans="1:12">
@@ -10517,13 +10628,13 @@
         <v>746</v>
       </c>
       <c r="E298" t="s">
+        <v>1190</v>
+      </c>
+      <c r="G298" t="s">
         <v>1191</v>
       </c>
-      <c r="G298" t="s">
+      <c r="L298" t="s">
         <v>1192</v>
-      </c>
-      <c r="L298" t="s">
-        <v>1193</v>
       </c>
     </row>
     <row r="299" spans="1:12">
@@ -10531,13 +10642,13 @@
         <v>746</v>
       </c>
       <c r="E299" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G299" t="s">
+        <v>1191</v>
+      </c>
+      <c r="L299" t="s">
         <v>1194</v>
-      </c>
-      <c r="G299" t="s">
-        <v>1192</v>
-      </c>
-      <c r="L299" t="s">
-        <v>1195</v>
       </c>
     </row>
     <row r="300" spans="1:12">
@@ -10545,13 +10656,13 @@
         <v>746</v>
       </c>
       <c r="E300" t="s">
+        <v>1195</v>
+      </c>
+      <c r="G300" t="s">
         <v>1196</v>
       </c>
-      <c r="G300" t="s">
+      <c r="L300" t="s">
         <v>1197</v>
-      </c>
-      <c r="L300" t="s">
-        <v>1198</v>
       </c>
     </row>
     <row r="301" spans="1:12">
@@ -10559,13 +10670,13 @@
         <v>746</v>
       </c>
       <c r="E301" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G301" t="s">
+        <v>1196</v>
+      </c>
+      <c r="L301" t="s">
         <v>1199</v>
-      </c>
-      <c r="G301" t="s">
-        <v>1197</v>
-      </c>
-      <c r="L301" t="s">
-        <v>1200</v>
       </c>
     </row>
     <row r="302" spans="1:12">
@@ -10573,13 +10684,13 @@
         <v>746</v>
       </c>
       <c r="E302" t="s">
+        <v>1200</v>
+      </c>
+      <c r="G302" t="s">
         <v>1201</v>
       </c>
-      <c r="G302" t="s">
+      <c r="L302" t="s">
         <v>1202</v>
-      </c>
-      <c r="L302" t="s">
-        <v>1203</v>
       </c>
     </row>
     <row r="303" spans="1:12">
@@ -10587,13 +10698,13 @@
         <v>746</v>
       </c>
       <c r="E303" t="s">
+        <v>1203</v>
+      </c>
+      <c r="G303" t="s">
+        <v>1201</v>
+      </c>
+      <c r="L303" t="s">
         <v>1204</v>
-      </c>
-      <c r="G303" t="s">
-        <v>1202</v>
-      </c>
-      <c r="L303" t="s">
-        <v>1205</v>
       </c>
     </row>
     <row r="304" spans="1:12">
@@ -10601,13 +10712,13 @@
         <v>746</v>
       </c>
       <c r="E304" t="s">
+        <v>1205</v>
+      </c>
+      <c r="G304" t="s">
         <v>1206</v>
       </c>
-      <c r="G304" t="s">
+      <c r="L304" t="s">
         <v>1207</v>
-      </c>
-      <c r="L304" t="s">
-        <v>1208</v>
       </c>
     </row>
     <row r="305" spans="1:12">
@@ -10615,13 +10726,13 @@
         <v>746</v>
       </c>
       <c r="E305" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G305" t="s">
         <v>1209</v>
       </c>
-      <c r="G305" t="s">
+      <c r="L305" t="s">
         <v>1210</v>
-      </c>
-      <c r="L305" t="s">
-        <v>1211</v>
       </c>
     </row>
     <row r="306" spans="1:12">
@@ -10629,13 +10740,13 @@
         <v>746</v>
       </c>
       <c r="E306" t="s">
+        <v>1211</v>
+      </c>
+      <c r="G306" t="s">
         <v>1212</v>
       </c>
-      <c r="G306" t="s">
+      <c r="L306" t="s">
         <v>1213</v>
-      </c>
-      <c r="L306" t="s">
-        <v>1214</v>
       </c>
     </row>
     <row r="307" spans="1:12">
@@ -10643,13 +10754,13 @@
         <v>746</v>
       </c>
       <c r="E307" t="s">
+        <v>1214</v>
+      </c>
+      <c r="G307" t="s">
         <v>1215</v>
       </c>
-      <c r="G307" t="s">
+      <c r="L307" t="s">
         <v>1216</v>
-      </c>
-      <c r="L307" t="s">
-        <v>1217</v>
       </c>
     </row>
     <row r="308" spans="1:12">
@@ -10657,13 +10768,13 @@
         <v>746</v>
       </c>
       <c r="E308" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="G308" t="s">
         <v>185</v>
       </c>
       <c r="L308" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="309" spans="1:12">
@@ -10671,13 +10782,13 @@
         <v>746</v>
       </c>
       <c r="E309" t="s">
+        <v>1219</v>
+      </c>
+      <c r="G309" t="s">
         <v>1220</v>
       </c>
-      <c r="G309" t="s">
+      <c r="L309" t="s">
         <v>1221</v>
-      </c>
-      <c r="L309" t="s">
-        <v>1222</v>
       </c>
     </row>
     <row r="310" spans="1:12">
@@ -10685,13 +10796,13 @@
         <v>746</v>
       </c>
       <c r="E310" t="s">
+        <v>1222</v>
+      </c>
+      <c r="G310" t="s">
+        <v>1220</v>
+      </c>
+      <c r="L310" t="s">
         <v>1223</v>
-      </c>
-      <c r="G310" t="s">
-        <v>1221</v>
-      </c>
-      <c r="L310" t="s">
-        <v>1224</v>
       </c>
     </row>
     <row r="311" spans="1:12">
@@ -10699,13 +10810,13 @@
         <v>746</v>
       </c>
       <c r="E311" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G311" t="s">
+        <v>1220</v>
+      </c>
+      <c r="L311" t="s">
         <v>1225</v>
-      </c>
-      <c r="G311" t="s">
-        <v>1221</v>
-      </c>
-      <c r="L311" t="s">
-        <v>1226</v>
       </c>
     </row>
     <row r="312" spans="1:12">
@@ -10713,13 +10824,13 @@
         <v>746</v>
       </c>
       <c r="E312" t="s">
+        <v>1226</v>
+      </c>
+      <c r="G312" t="s">
+        <v>1220</v>
+      </c>
+      <c r="L312" t="s">
         <v>1227</v>
-      </c>
-      <c r="G312" t="s">
-        <v>1221</v>
-      </c>
-      <c r="L312" t="s">
-        <v>1228</v>
       </c>
     </row>
     <row r="313" spans="1:12">
@@ -10727,13 +10838,13 @@
         <v>746</v>
       </c>
       <c r="E313" t="s">
+        <v>1228</v>
+      </c>
+      <c r="G313" t="s">
+        <v>1220</v>
+      </c>
+      <c r="L313" t="s">
         <v>1229</v>
-      </c>
-      <c r="G313" t="s">
-        <v>1221</v>
-      </c>
-      <c r="L313" t="s">
-        <v>1230</v>
       </c>
     </row>
     <row r="314" spans="1:12">
@@ -10741,13 +10852,13 @@
         <v>746</v>
       </c>
       <c r="E314" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G314" t="s">
+        <v>1220</v>
+      </c>
+      <c r="L314" t="s">
         <v>1231</v>
-      </c>
-      <c r="G314" t="s">
-        <v>1221</v>
-      </c>
-      <c r="L314" t="s">
-        <v>1232</v>
       </c>
     </row>
     <row r="315" spans="1:12">
@@ -10755,13 +10866,13 @@
         <v>746</v>
       </c>
       <c r="E315" t="s">
+        <v>1232</v>
+      </c>
+      <c r="G315" t="s">
+        <v>1220</v>
+      </c>
+      <c r="L315" t="s">
         <v>1233</v>
-      </c>
-      <c r="G315" t="s">
-        <v>1221</v>
-      </c>
-      <c r="L315" t="s">
-        <v>1234</v>
       </c>
     </row>
     <row r="316" spans="1:12">
@@ -10769,13 +10880,13 @@
         <v>746</v>
       </c>
       <c r="E316" t="s">
+        <v>1234</v>
+      </c>
+      <c r="G316" t="s">
         <v>1235</v>
       </c>
-      <c r="G316" t="s">
+      <c r="L316" t="s">
         <v>1236</v>
-      </c>
-      <c r="L316" t="s">
-        <v>1237</v>
       </c>
     </row>
     <row r="317" spans="1:12">
@@ -10783,13 +10894,13 @@
         <v>746</v>
       </c>
       <c r="E317" t="s">
+        <v>1237</v>
+      </c>
+      <c r="G317" t="s">
+        <v>1235</v>
+      </c>
+      <c r="L317" t="s">
         <v>1238</v>
-      </c>
-      <c r="G317" t="s">
-        <v>1236</v>
-      </c>
-      <c r="L317" t="s">
-        <v>1239</v>
       </c>
     </row>
     <row r="318" spans="1:12">
@@ -10797,13 +10908,13 @@
         <v>746</v>
       </c>
       <c r="E318" t="s">
+        <v>1239</v>
+      </c>
+      <c r="G318" t="s">
+        <v>1235</v>
+      </c>
+      <c r="L318" t="s">
         <v>1240</v>
-      </c>
-      <c r="G318" t="s">
-        <v>1236</v>
-      </c>
-      <c r="L318" t="s">
-        <v>1241</v>
       </c>
     </row>
     <row r="319" spans="1:12">
@@ -10811,13 +10922,13 @@
         <v>746</v>
       </c>
       <c r="E319" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G319" t="s">
+        <v>1235</v>
+      </c>
+      <c r="L319" t="s">
         <v>1242</v>
-      </c>
-      <c r="G319" t="s">
-        <v>1236</v>
-      </c>
-      <c r="L319" t="s">
-        <v>1243</v>
       </c>
     </row>
     <row r="320" spans="1:12">
@@ -10825,13 +10936,13 @@
         <v>746</v>
       </c>
       <c r="E320" t="s">
+        <v>1243</v>
+      </c>
+      <c r="G320" t="s">
+        <v>1235</v>
+      </c>
+      <c r="L320" t="s">
         <v>1244</v>
-      </c>
-      <c r="G320" t="s">
-        <v>1236</v>
-      </c>
-      <c r="L320" t="s">
-        <v>1245</v>
       </c>
     </row>
     <row r="321" spans="1:12">
@@ -10839,13 +10950,13 @@
         <v>746</v>
       </c>
       <c r="E321" t="s">
+        <v>1245</v>
+      </c>
+      <c r="G321" t="s">
+        <v>1235</v>
+      </c>
+      <c r="L321" t="s">
         <v>1246</v>
-      </c>
-      <c r="G321" t="s">
-        <v>1236</v>
-      </c>
-      <c r="L321" t="s">
-        <v>1247</v>
       </c>
     </row>
     <row r="322" spans="1:12">
@@ -10853,13 +10964,13 @@
         <v>746</v>
       </c>
       <c r="E322" t="s">
+        <v>1247</v>
+      </c>
+      <c r="G322" t="s">
+        <v>1235</v>
+      </c>
+      <c r="L322" t="s">
         <v>1248</v>
-      </c>
-      <c r="G322" t="s">
-        <v>1236</v>
-      </c>
-      <c r="L322" t="s">
-        <v>1249</v>
       </c>
     </row>
     <row r="323" spans="1:12">
@@ -10867,13 +10978,13 @@
         <v>746</v>
       </c>
       <c r="E323" t="s">
+        <v>1249</v>
+      </c>
+      <c r="G323" t="s">
         <v>1250</v>
       </c>
-      <c r="G323" t="s">
+      <c r="L323" t="s">
         <v>1251</v>
-      </c>
-      <c r="L323" t="s">
-        <v>1252</v>
       </c>
     </row>
     <row r="324" spans="1:12">
@@ -10881,13 +10992,13 @@
         <v>746</v>
       </c>
       <c r="E324" t="s">
+        <v>1252</v>
+      </c>
+      <c r="G324" t="s">
+        <v>1250</v>
+      </c>
+      <c r="L324" t="s">
         <v>1253</v>
-      </c>
-      <c r="G324" t="s">
-        <v>1251</v>
-      </c>
-      <c r="L324" t="s">
-        <v>1254</v>
       </c>
     </row>
     <row r="325" spans="1:12">
@@ -10895,13 +11006,13 @@
         <v>746</v>
       </c>
       <c r="E325" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="G325" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="L325" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="326" spans="1:12">
@@ -10909,13 +11020,13 @@
         <v>746</v>
       </c>
       <c r="E326" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G326" t="s">
         <v>1256</v>
       </c>
-      <c r="G326" t="s">
+      <c r="L326" t="s">
         <v>1257</v>
-      </c>
-      <c r="L326" t="s">
-        <v>1258</v>
       </c>
     </row>
     <row r="327" spans="1:12">
@@ -10923,13 +11034,13 @@
         <v>746</v>
       </c>
       <c r="E327" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="G327" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="L327" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="328" spans="1:12">
@@ -10937,13 +11048,13 @@
         <v>746</v>
       </c>
       <c r="E328" t="s">
+        <v>1259</v>
+      </c>
+      <c r="G328" t="s">
+        <v>1256</v>
+      </c>
+      <c r="L328" t="s">
         <v>1260</v>
-      </c>
-      <c r="G328" t="s">
-        <v>1257</v>
-      </c>
-      <c r="L328" t="s">
-        <v>1261</v>
       </c>
     </row>
     <row r="329" spans="1:12">
@@ -10951,21 +11062,24 @@
         <v>746</v>
       </c>
       <c r="E329" t="s">
+        <v>1261</v>
+      </c>
+      <c r="G329" t="s">
+        <v>1256</v>
+      </c>
+      <c r="L329" t="s">
         <v>1262</v>
       </c>
-      <c r="G329" t="s">
-        <v>1257</v>
-      </c>
-      <c r="L329" t="s">
+    </row>
+    <row r="330" spans="1:12" ht="16">
+      <c r="A330" t="s">
+        <v>746</v>
+      </c>
+      <c r="C330" s="6" t="s">
+        <v>1431</v>
+      </c>
+      <c r="E330" t="s">
         <v>1263</v>
-      </c>
-    </row>
-    <row r="330" spans="1:12">
-      <c r="A330" t="s">
-        <v>746</v>
-      </c>
-      <c r="E330" t="s">
-        <v>1264</v>
       </c>
       <c r="G330" t="s">
         <v>883</v>
@@ -10979,13 +11093,13 @@
         <v>746</v>
       </c>
       <c r="E331" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G331" t="s">
         <v>1265</v>
       </c>
-      <c r="G331" t="s">
+      <c r="L331" t="s">
         <v>1266</v>
-      </c>
-      <c r="L331" t="s">
-        <v>1267</v>
       </c>
     </row>
     <row r="332" spans="1:12">
@@ -10993,13 +11107,13 @@
         <v>746</v>
       </c>
       <c r="E332" t="s">
+        <v>1267</v>
+      </c>
+      <c r="G332" t="s">
         <v>1268</v>
       </c>
-      <c r="G332" t="s">
+      <c r="L332" t="s">
         <v>1269</v>
-      </c>
-      <c r="L332" t="s">
-        <v>1270</v>
       </c>
     </row>
     <row r="333" spans="1:12">
@@ -11007,10 +11121,10 @@
         <v>746</v>
       </c>
       <c r="E333" t="s">
+        <v>1270</v>
+      </c>
+      <c r="G333" t="s">
         <v>1271</v>
-      </c>
-      <c r="G333" t="s">
-        <v>1272</v>
       </c>
       <c r="L333" t="s">
         <v>840</v>
@@ -11021,13 +11135,13 @@
         <v>746</v>
       </c>
       <c r="E334" t="s">
+        <v>1272</v>
+      </c>
+      <c r="G334" t="s">
         <v>1273</v>
       </c>
-      <c r="G334" t="s">
+      <c r="L334" t="s">
         <v>1274</v>
-      </c>
-      <c r="L334" t="s">
-        <v>1275</v>
       </c>
     </row>
     <row r="335" spans="1:12">
@@ -11049,7 +11163,7 @@
         <v>746</v>
       </c>
       <c r="E336" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="G336" t="s">
         <v>759</v>
@@ -11063,27 +11177,30 @@
         <v>746</v>
       </c>
       <c r="E337" t="s">
+        <v>1276</v>
+      </c>
+      <c r="G337" t="s">
         <v>1277</v>
       </c>
-      <c r="G337" t="s">
+      <c r="L337" t="s">
         <v>1278</v>
-      </c>
-      <c r="L337" t="s">
-        <v>1279</v>
       </c>
     </row>
     <row r="338" spans="1:12">
       <c r="A338" t="s">
         <v>746</v>
       </c>
+      <c r="C338" s="7" t="s">
+        <v>1432</v>
+      </c>
       <c r="E338" t="s">
+        <v>1279</v>
+      </c>
+      <c r="G338" t="s">
         <v>1280</v>
       </c>
-      <c r="G338" t="s">
+      <c r="L338" t="s">
         <v>1281</v>
-      </c>
-      <c r="L338" t="s">
-        <v>1282</v>
       </c>
     </row>
     <row r="339" spans="1:12">
@@ -11091,10 +11208,10 @@
         <v>746</v>
       </c>
       <c r="E339" t="s">
+        <v>1282</v>
+      </c>
+      <c r="G339" t="s">
         <v>1283</v>
-      </c>
-      <c r="G339" t="s">
-        <v>1284</v>
       </c>
       <c r="L339" t="s">
         <v>995</v>
@@ -11105,38 +11222,44 @@
         <v>746</v>
       </c>
       <c r="E340" t="s">
+        <v>1284</v>
+      </c>
+      <c r="G340" t="s">
+        <v>1283</v>
+      </c>
+      <c r="L340" t="s">
         <v>1285</v>
-      </c>
-      <c r="G340" t="s">
-        <v>1284</v>
-      </c>
-      <c r="L340" t="s">
-        <v>1286</v>
       </c>
     </row>
     <row r="341" spans="1:12">
       <c r="A341" t="s">
         <v>746</v>
       </c>
+      <c r="C341" t="s">
+        <v>1433</v>
+      </c>
       <c r="E341" t="s">
+        <v>1286</v>
+      </c>
+      <c r="G341" t="s">
         <v>1287</v>
       </c>
-      <c r="G341" t="s">
+      <c r="L341" t="s">
         <v>1288</v>
-      </c>
-      <c r="L341" t="s">
-        <v>1289</v>
       </c>
     </row>
     <row r="342" spans="1:12">
       <c r="A342" t="s">
         <v>746</v>
       </c>
+      <c r="C342" s="7" t="s">
+        <v>1434</v>
+      </c>
       <c r="E342" t="s">
+        <v>1289</v>
+      </c>
+      <c r="G342" t="s">
         <v>1290</v>
-      </c>
-      <c r="G342" t="s">
-        <v>1291</v>
       </c>
       <c r="L342" t="s">
         <v>1007</v>
@@ -11146,28 +11269,34 @@
       <c r="A343" t="s">
         <v>746</v>
       </c>
+      <c r="C343" t="s">
+        <v>1435</v>
+      </c>
       <c r="E343" t="s">
+        <v>1291</v>
+      </c>
+      <c r="G343" t="s">
         <v>1292</v>
       </c>
-      <c r="G343" t="s">
+      <c r="L343" t="s">
         <v>1293</v>
-      </c>
-      <c r="L343" t="s">
-        <v>1294</v>
       </c>
     </row>
     <row r="344" spans="1:12">
       <c r="A344" t="s">
         <v>746</v>
       </c>
+      <c r="C344" t="s">
+        <v>1436</v>
+      </c>
       <c r="E344" t="s">
+        <v>1294</v>
+      </c>
+      <c r="G344" t="s">
         <v>1295</v>
       </c>
-      <c r="G344" t="s">
+      <c r="L344" t="s">
         <v>1296</v>
-      </c>
-      <c r="L344" t="s">
-        <v>1297</v>
       </c>
     </row>
     <row r="345" spans="1:12">
@@ -11175,13 +11304,13 @@
         <v>746</v>
       </c>
       <c r="E345" t="s">
+        <v>1297</v>
+      </c>
+      <c r="G345" t="s">
         <v>1298</v>
       </c>
-      <c r="G345" t="s">
+      <c r="L345" t="s">
         <v>1299</v>
-      </c>
-      <c r="L345" t="s">
-        <v>1300</v>
       </c>
     </row>
     <row r="346" spans="1:12">
@@ -11189,13 +11318,13 @@
         <v>746</v>
       </c>
       <c r="E346" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="G346" t="s">
         <v>17</v>
       </c>
       <c r="L346" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="347" spans="1:12">
@@ -11203,13 +11332,13 @@
         <v>746</v>
       </c>
       <c r="E347" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="G347" t="s">
         <v>17</v>
       </c>
       <c r="L347" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="348" spans="1:12">
@@ -11217,13 +11346,13 @@
         <v>746</v>
       </c>
       <c r="E348" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="G348" t="s">
         <v>17</v>
       </c>
       <c r="L348" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="349" spans="1:12">
@@ -11231,13 +11360,13 @@
         <v>746</v>
       </c>
       <c r="E349" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="G349" t="s">
         <v>26</v>
       </c>
       <c r="L349" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="350" spans="1:12">
@@ -11245,13 +11374,13 @@
         <v>746</v>
       </c>
       <c r="E350" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="G350" t="s">
         <v>26</v>
       </c>
       <c r="L350" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="351" spans="1:12">
@@ -11259,10 +11388,10 @@
         <v>746</v>
       </c>
       <c r="E351" t="s">
+        <v>1310</v>
+      </c>
+      <c r="G351" t="s">
         <v>1311</v>
-      </c>
-      <c r="G351" t="s">
-        <v>1312</v>
       </c>
       <c r="L351" t="s">
         <v>995</v>
@@ -11273,10 +11402,10 @@
         <v>746</v>
       </c>
       <c r="E352" t="s">
+        <v>1312</v>
+      </c>
+      <c r="G352" t="s">
         <v>1313</v>
-      </c>
-      <c r="G352" t="s">
-        <v>1314</v>
       </c>
       <c r="L352" t="s">
         <v>753</v>
@@ -11287,38 +11416,44 @@
         <v>746</v>
       </c>
       <c r="E353" t="s">
+        <v>1314</v>
+      </c>
+      <c r="G353" t="s">
         <v>1315</v>
       </c>
-      <c r="G353" t="s">
+      <c r="L353" t="s">
         <v>1316</v>
-      </c>
-      <c r="L353" t="s">
-        <v>1317</v>
       </c>
     </row>
     <row r="354" spans="1:12">
       <c r="A354" t="s">
         <v>746</v>
       </c>
+      <c r="C354" t="s">
+        <v>1439</v>
+      </c>
       <c r="E354" t="s">
+        <v>1317</v>
+      </c>
+      <c r="G354" t="s">
+        <v>1438</v>
+      </c>
+      <c r="L354" t="s">
         <v>1318</v>
-      </c>
-      <c r="G354" t="s">
-        <v>1319</v>
-      </c>
-      <c r="L354" t="s">
-        <v>1320</v>
       </c>
     </row>
     <row r="355" spans="1:12">
       <c r="A355" t="s">
         <v>746</v>
       </c>
+      <c r="C355" s="7" t="s">
+        <v>1437</v>
+      </c>
       <c r="E355" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="G355" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="L355" t="s">
         <v>766</v>
@@ -11326,299 +11461,299 @@
     </row>
     <row r="356" spans="1:12">
       <c r="A356" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C356" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D356" t="s">
         <v>1323</v>
-      </c>
-      <c r="C356" t="s">
-        <v>1324</v>
-      </c>
-      <c r="D356" t="s">
-        <v>1325</v>
       </c>
       <c r="G356">
         <v>5</v>
       </c>
       <c r="L356" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="357" spans="1:12">
       <c r="A357" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C357" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="D357" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="G357">
         <v>6</v>
       </c>
       <c r="L357" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="358" spans="1:12">
       <c r="A358" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C358" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="D358" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="G358">
         <v>9</v>
       </c>
       <c r="L358" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="359" spans="1:12">
       <c r="A359" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C359" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
       <c r="D359" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="G359">
         <v>13</v>
       </c>
       <c r="L359" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="360" spans="1:12">
       <c r="A360" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C360" t="s">
+        <v>1335</v>
+      </c>
+      <c r="D360" t="s">
         <v>1336</v>
-      </c>
-      <c r="C360" t="s">
-        <v>1337</v>
-      </c>
-      <c r="D360" t="s">
-        <v>1338</v>
       </c>
       <c r="G360">
         <v>7</v>
       </c>
       <c r="L360" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="361" spans="1:12">
       <c r="A361" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C361" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="D361" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="G361">
         <v>11</v>
       </c>
       <c r="L361" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="362" spans="1:12">
       <c r="A362" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C362" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="D362" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="G362" t="s">
         <v>17</v>
       </c>
       <c r="L362" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="363" spans="1:12">
       <c r="A363" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C363" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D363" t="s">
         <v>1346</v>
       </c>
-      <c r="C363" t="s">
+      <c r="L363" t="s">
         <v>1347</v>
-      </c>
-      <c r="D363" t="s">
-        <v>1348</v>
-      </c>
-      <c r="L363" t="s">
-        <v>1349</v>
       </c>
     </row>
     <row r="364" spans="1:12">
       <c r="A364" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C364" t="s">
+        <v>1349</v>
+      </c>
+      <c r="D364" t="s">
         <v>1350</v>
-      </c>
-      <c r="C364" t="s">
-        <v>1351</v>
-      </c>
-      <c r="D364" t="s">
-        <v>1352</v>
       </c>
       <c r="G364">
         <v>4</v>
       </c>
       <c r="L364" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="365" spans="1:12">
       <c r="A365" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C365" t="s">
-        <v>1354</v>
+        <v>1352</v>
       </c>
       <c r="D365" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="G365">
         <v>16</v>
       </c>
       <c r="L365" t="s">
-        <v>1356</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="366" spans="1:12">
       <c r="A366" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C366" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="D366" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="G366">
         <v>17</v>
       </c>
       <c r="L366" t="s">
-        <v>1359</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="367" spans="1:12">
       <c r="A367" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C367" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D367" t="s">
         <v>1360</v>
-      </c>
-      <c r="C367" t="s">
-        <v>1361</v>
-      </c>
-      <c r="D367" t="s">
-        <v>1362</v>
       </c>
       <c r="G367">
         <v>6</v>
       </c>
       <c r="L367" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="368" spans="1:12">
       <c r="A368" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C368" t="s">
-        <v>1364</v>
+        <v>1362</v>
       </c>
       <c r="D368" t="s">
-        <v>1365</v>
+        <v>1363</v>
       </c>
       <c r="G368">
         <v>8</v>
       </c>
       <c r="L368" t="s">
-        <v>1366</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="369" spans="1:12">
       <c r="A369" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="C369" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="D369" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="G369">
         <v>8</v>
       </c>
       <c r="L369" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="370" spans="1:12">
       <c r="A370" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="C370" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="D370" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="G370">
         <v>13</v>
       </c>
       <c r="L370" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="371" spans="1:12">
       <c r="A371" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="C371" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="D371" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="G371">
         <v>12</v>
       </c>
       <c r="L371" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="372" spans="1:12">
       <c r="A372" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="C372" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="D372" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="G372">
         <v>11</v>
       </c>
       <c r="L372" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="373" spans="1:12">
       <c r="A373" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="C373" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="D373" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="G373">
         <v>5</v>
@@ -11629,30 +11764,30 @@
     </row>
     <row r="374" spans="1:12">
       <c r="A374" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="C374" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="D374" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="G374">
         <v>10</v>
       </c>
       <c r="L374" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="375" spans="1:12">
       <c r="A375" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="C375" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="D375" t="s">
-        <v>1385</v>
+        <v>1383</v>
       </c>
       <c r="G375">
         <v>4</v>
@@ -11663,209 +11798,259 @@
     </row>
     <row r="376" spans="1:12">
       <c r="A376" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="C376" t="s">
-        <v>1386</v>
+        <v>1384</v>
       </c>
       <c r="D376" t="s">
-        <v>1387</v>
+        <v>1385</v>
       </c>
       <c r="G376">
         <v>2</v>
       </c>
       <c r="L376" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="377" spans="1:12">
       <c r="A377" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C377" t="s">
-        <v>1389</v>
+        <v>1387</v>
       </c>
       <c r="D377" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="G377">
         <v>12</v>
       </c>
       <c r="L377" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="378" spans="1:12">
       <c r="A378" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C378" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="D378" t="s">
-        <v>1393</v>
+        <v>1391</v>
       </c>
       <c r="G378">
         <v>3</v>
       </c>
       <c r="L378" t="s">
-        <v>1394</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="379" spans="1:12">
       <c r="A379" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C379" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="D379" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="G379">
         <v>14</v>
       </c>
       <c r="L379" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="380" spans="1:12">
       <c r="A380" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C380" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="D380" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="G380">
         <v>7</v>
       </c>
       <c r="L380" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="381" spans="1:12">
       <c r="A381" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C381" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="D381" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="G381">
         <v>15</v>
       </c>
       <c r="L381" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="382" spans="1:12">
       <c r="A382" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="C382" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="D382" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="G382">
         <v>3</v>
       </c>
       <c r="L382" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="383" spans="1:12">
       <c r="A383" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="C383" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="D383" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="G383">
         <v>9</v>
       </c>
       <c r="L383" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="384" spans="1:12">
       <c r="A384" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="C384" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="D384" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="G384">
         <v>2</v>
       </c>
       <c r="L384" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="385" spans="1:14">
+      <c r="A385" t="s">
         <v>1412</v>
       </c>
-    </row>
-    <row r="385" spans="1:12">
-      <c r="A385" t="s">
+      <c r="B385" t="s">
         <v>1414</v>
       </c>
-      <c r="B385" t="s">
-        <v>1416</v>
-      </c>
       <c r="C385" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="D385" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="G385" t="s">
         <v>87</v>
       </c>
       <c r="L385" s="3" t="s">
-        <v>1415</v>
-      </c>
-    </row>
-    <row r="386" spans="1:12">
+        <v>1413</v>
+      </c>
+      <c r="M385" s="7">
+        <v>10400585</v>
+      </c>
+      <c r="N385">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386" spans="1:14">
       <c r="A386" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B386" t="s">
         <v>1419</v>
       </c>
-      <c r="B386" t="s">
+      <c r="C386" t="s">
+        <v>1416</v>
+      </c>
+      <c r="G386" t="s">
+        <v>1418</v>
+      </c>
+      <c r="L386" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="387" spans="1:14">
+      <c r="A387" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C387" s="4" t="s">
         <v>1421</v>
       </c>
-      <c r="C386" t="s">
-        <v>1418</v>
-      </c>
-      <c r="G386" t="s">
-        <v>1420</v>
-      </c>
-      <c r="L386" t="s">
+      <c r="G387" t="s">
+        <v>1209</v>
+      </c>
+      <c r="L387" t="s">
         <v>1422</v>
       </c>
     </row>
-    <row r="387" spans="1:12">
-      <c r="A387" t="s">
-        <v>1336</v>
-      </c>
-      <c r="C387" s="4" t="s">
-        <v>1423</v>
-      </c>
-      <c r="G387" t="s">
-        <v>1210</v>
-      </c>
-      <c r="L387" t="s">
-        <v>1424</v>
+    <row r="388" spans="1:14">
+      <c r="A388" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C388" s="7" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D388" t="s">
+        <v>1426</v>
+      </c>
+      <c r="L388" t="s">
+        <v>1427</v>
+      </c>
+      <c r="M388" s="7">
+        <v>8566816</v>
+      </c>
+    </row>
+    <row r="389" spans="1:14">
+      <c r="A389" t="s">
+        <v>1412</v>
+      </c>
+      <c r="C389" s="7" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D389" t="s">
+        <v>1428</v>
+      </c>
+      <c r="L389" s="9" t="s">
+        <v>1430</v>
+      </c>
+      <c r="M389" s="7">
+        <v>7565115</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M385" r:id="rId1" display="https://www.ncbi.nlm.nih.gov/pubmed/10400585" xr:uid="{661D96EC-7924-2E41-8D03-815653E6C6AA}"/>
+    <hyperlink ref="C388" r:id="rId2" display="https://www.ncbi.nlm.nih.gov/protein/847945" xr:uid="{DF9EE5E9-70FB-7F41-9D44-2EE74E7411D7}"/>
+    <hyperlink ref="M388" r:id="rId3" display="https://www.ncbi.nlm.nih.gov/pubmed/8566816" xr:uid="{DBAEA4EA-AF64-BA49-8A2F-81653C5ED580}"/>
+    <hyperlink ref="C389" r:id="rId4" display="https://www.ncbi.nlm.nih.gov/protein/1545852" xr:uid="{F17FBAB1-A81B-CA4F-99A5-30B7DF20FCE2}"/>
+    <hyperlink ref="M389" r:id="rId5" display="https://www.ncbi.nlm.nih.gov/pubmed/7565115" xr:uid="{14F1C977-2322-3A48-AED0-B932E4C3D0AC}"/>
+    <hyperlink ref="C338" r:id="rId6" tooltip="Show report for WP_074526664.1" display="https://www.ncbi.nlm.nih.gov/protein/WP_074526664.1?report=genbank&amp;log$=prottop&amp;blast_rank=1&amp;RID=YZE93SS0013" xr:uid="{26868CDD-EF4B-A242-9570-D31ADE7AD9F0}"/>
+    <hyperlink ref="C342" r:id="rId7" tooltip="Show report for WP_024244058.1" display="https://www.ncbi.nlm.nih.gov/protein/WP_024244058.1?report=genbank&amp;log$=prottop&amp;blast_rank=1&amp;RID=YZEEMGHR016" xr:uid="{BFC7435A-35BA-854A-BF8A-8DEF7A54AA1E}"/>
+    <hyperlink ref="C355" r:id="rId8" tooltip="Show report for WP_000549530.1" display="https://www.ncbi.nlm.nih.gov/protein/WP_000549530.1?report=genbank&amp;log$=prottop&amp;blast_rank=1&amp;RID=YZEUVX5D013" xr:uid="{D2F05105-38B7-BF4C-A9D4-4FB3059DDCE3}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>